<commit_message>
linear regression w/ quadratic trend + sine/cosine
</commit_message>
<xml_diff>
--- a/storage_forecast/storage.xlsx
+++ b/storage_forecast/storage.xlsx
@@ -1764,11 +1764,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C468"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="C279" sqref="C279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -1943,7 +1947,7 @@
         <v>18</v>
       </c>
       <c r="C16" s="1">
-        <v>20457.891</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1998,7 +2002,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="1">
-        <v>22025.895</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3296,7 +3300,7 @@
         <v>141</v>
       </c>
       <c r="C139" s="1">
-        <v>33532.008000000002</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="140" spans="1:3">
@@ -4451,7 +4455,7 @@
         <v>246</v>
       </c>
       <c r="C244" s="1">
-        <v>49424.385000000002</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="245" spans="1:3">
@@ -4825,7 +4829,7 @@
         <v>280</v>
       </c>
       <c r="C278" s="1">
-        <v>54484.197999999997</v>
+        <v>340000</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -5441,7 +5445,7 @@
         <v>336</v>
       </c>
       <c r="C334" s="1">
-        <v>68086.093999999997</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="335" spans="1:3">
@@ -6772,7 +6776,7 @@
         <v>457</v>
       </c>
       <c r="C455" s="1">
-        <v>183141.87700000001</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="456" spans="1:3">

</xml_diff>